<commit_message>
10.11.2015 - added init load ui
</commit_message>
<xml_diff>
--- a/ScreenDensity.xlsx
+++ b/ScreenDensity.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="360" yWindow="45" windowWidth="21015" windowHeight="9975"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="расчеты" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>small</t>
   </si>
@@ -55,6 +56,69 @@
   </si>
   <si>
     <t>%-answer</t>
+  </si>
+  <si>
+    <t>width-dp</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Фильтр первого уровня</t>
+  </si>
+  <si>
+    <t>Фильтр второго уровня</t>
+  </si>
+  <si>
+    <t>Локаль</t>
+  </si>
+  <si>
+    <t>Сохранение данных в файл</t>
+  </si>
+  <si>
+    <t>Обработка ошибок</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>корзина</t>
+  </si>
+  <si>
+    <t>регистрация</t>
+  </si>
+  <si>
+    <t>вход</t>
+  </si>
+  <si>
+    <t>локаль</t>
+  </si>
+  <si>
+    <t>страна</t>
+  </si>
+  <si>
+    <t>город</t>
+  </si>
+  <si>
+    <t>данные для входа</t>
+  </si>
+  <si>
+    <t>смена названий при клике на поле из выпадающего списка</t>
+  </si>
+  <si>
+    <t>отсутствие интернета</t>
+  </si>
+  <si>
+    <t>сформировать string.xml</t>
+  </si>
+  <si>
+    <t>нет дизайна</t>
+  </si>
+  <si>
+    <t>фильтр второго уровня</t>
   </si>
 </sst>
 </file>
@@ -79,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,11 +151,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -101,6 +180,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,30 +487,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D1:P4"/>
+  <dimension ref="D2:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="10" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:16">
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="4:16">
+    <row r="2" spans="4:14">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,32 +518,26 @@
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="4:16">
+    <row r="3" spans="4:14">
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
@@ -470,39 +550,292 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
+        <v>640</v>
+      </c>
+      <c r="J3" s="1">
         <v>480</v>
       </c>
-      <c r="J3" s="1">
-        <v>100</v>
-      </c>
       <c r="K3" s="1">
+        <v>100</v>
+      </c>
+      <c r="L3" s="4">
+        <f>N3*I3/100</f>
+        <v>474.66666666666674</v>
+      </c>
+      <c r="M3" s="1">
         <v>356</v>
       </c>
-      <c r="P3" s="1">
-        <f>K3*J3/I3</f>
+      <c r="N3" s="1">
+        <f>M3*K3/J3</f>
         <v>74.166666666666671</v>
       </c>
     </row>
-    <row r="4" spans="4:16">
-      <c r="I4" s="1">
+    <row r="4" spans="4:14">
+      <c r="I4" s="3">
+        <v>360</v>
+      </c>
+      <c r="J4" s="1">
         <v>385</v>
       </c>
-      <c r="J4" s="1">
-        <v>100</v>
-      </c>
       <c r="K4" s="1">
+        <v>100</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4" si="0">N4*I4/100</f>
+        <v>332.88311688311688</v>
+      </c>
+      <c r="M4" s="1">
         <v>356</v>
       </c>
-      <c r="P4" s="1">
-        <f>K4*J4/I4</f>
+      <c r="N4" s="1">
+        <f>M4*K4/J4</f>
         <v>92.467532467532465</v>
       </c>
     </row>
+    <row r="5" spans="4:14">
+      <c r="I5" s="3">
+        <v>360</v>
+      </c>
+      <c r="J5" s="3">
+        <v>385</v>
+      </c>
+      <c r="K5" s="3">
+        <v>100</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L14" si="1">N5*I5/100</f>
+        <v>333.81818181818181</v>
+      </c>
+      <c r="M5" s="3">
+        <v>357</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ref="N5:N14" si="2">M5*K5/J5</f>
+        <v>92.727272727272734</v>
+      </c>
+    </row>
+    <row r="6" spans="4:14">
+      <c r="I6" s="3">
+        <v>360</v>
+      </c>
+      <c r="J6" s="3">
+        <v>385</v>
+      </c>
+      <c r="K6" s="3">
+        <v>100</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>334.7532467532468</v>
+      </c>
+      <c r="M6" s="3">
+        <v>358</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="2"/>
+        <v>92.987012987012989</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="I7" s="3">
+        <v>360</v>
+      </c>
+      <c r="J7" s="3">
+        <v>385</v>
+      </c>
+      <c r="K7" s="3">
+        <v>100</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>335.68831168831167</v>
+      </c>
+      <c r="M7" s="3">
+        <v>359</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="2"/>
+        <v>93.246753246753244</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14">
+      <c r="I8" s="3">
+        <v>360</v>
+      </c>
+      <c r="J8" s="3">
+        <v>385</v>
+      </c>
+      <c r="K8" s="3">
+        <v>100</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="1"/>
+        <v>336.62337662337666</v>
+      </c>
+      <c r="M8" s="3">
+        <v>360</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="2"/>
+        <v>93.506493506493513</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14">
+      <c r="I9" s="3">
+        <v>360</v>
+      </c>
+      <c r="J9" s="3">
+        <v>385</v>
+      </c>
+      <c r="K9" s="3">
+        <v>100</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="1"/>
+        <v>337.55844155844153</v>
+      </c>
+      <c r="M9" s="3">
+        <v>361</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="2"/>
+        <v>93.766233766233768</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14">
+      <c r="I10" s="3">
+        <v>360</v>
+      </c>
+      <c r="J10" s="3">
+        <v>385</v>
+      </c>
+      <c r="K10" s="3">
+        <v>100</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="1"/>
+        <v>338.49350649350652</v>
+      </c>
+      <c r="M10" s="3">
+        <v>362</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="2"/>
+        <v>94.025974025974023</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14">
+      <c r="I11" s="3">
+        <v>360</v>
+      </c>
+      <c r="J11" s="3">
+        <v>385</v>
+      </c>
+      <c r="K11" s="3">
+        <v>100</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="1"/>
+        <v>339.42857142857144</v>
+      </c>
+      <c r="M11" s="3">
+        <v>363</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="2"/>
+        <v>94.285714285714292</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="I12" s="3">
+        <v>360</v>
+      </c>
+      <c r="J12" s="3">
+        <v>385</v>
+      </c>
+      <c r="K12" s="3">
+        <v>100</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="1"/>
+        <v>340.36363636363637</v>
+      </c>
+      <c r="M12" s="3">
+        <v>364</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="2"/>
+        <v>94.545454545454547</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14">
+      <c r="I13" s="3">
+        <v>640</v>
+      </c>
+      <c r="J13" s="3">
+        <v>720</v>
+      </c>
+      <c r="K13" s="3">
+        <v>100</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="1"/>
+        <v>244.44444444444446</v>
+      </c>
+      <c r="M13" s="3">
+        <v>275</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="2"/>
+        <v>38.194444444444443</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14">
+      <c r="I14" s="3">
+        <v>360</v>
+      </c>
+      <c r="J14" s="3">
+        <v>480</v>
+      </c>
+      <c r="K14" s="3">
+        <v>100</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="1"/>
+        <v>206.25</v>
+      </c>
+      <c r="M14" s="3">
+        <v>275</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="2"/>
+        <v>57.291666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14">
+      <c r="I16" s="3">
+        <v>330</v>
+      </c>
+      <c r="J16" s="1">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1">
+        <v>375</v>
+      </c>
+      <c r="L16" s="4">
+        <f>K16*J16/I16</f>
+        <v>113.63636363636364</v>
+      </c>
+      <c r="M16" s="1">
+        <v>337</v>
+      </c>
+      <c r="N16" s="1">
+        <f>L16*M16/J16</f>
+        <v>382.95454545454544</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="L1:O1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -510,13 +843,265 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="16.7109375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>